<commit_message>
Converting resume files to text
</commit_message>
<xml_diff>
--- a/data/JDs.xlsx
+++ b/data/JDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\om\code\Resume-Evaluator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A2371-9324-4E3E-81A1-9CBB6A058046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2327CB0-C07D-40A1-B954-DAF29290DC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3972,11 +3972,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4259,8 +4256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4276,963 +4273,963 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>44</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>44</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>64</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>64</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>64</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>64</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>64</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>64</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>64</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>64</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>85</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>85</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>85</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>85</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>85</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>85</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>85</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>106</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>106</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>106</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>106</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>106</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>106</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>106</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>106</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>106</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>106</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>106</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>106</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>106</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>